<commit_message>
feat/bug fix (total Label)
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Salgueir\Documents\GitHub\Budget-Manager-PY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bilha\Documents\GitHub\Budget-Manager-PY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB850F0-0CF9-4598-8C33-59B4F29E663C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34129A5B-000B-4B35-A073-D04DAC29B0A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -429,15 +429,78 @@
     <xf numFmtId="165" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -447,71 +510,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,7 +818,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="56.25" customHeight="1">
-      <c r="A1" s="8"/>
+      <c r="A1" s="31"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -827,33 +827,33 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="35">
         <v>45321</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A3" s="12"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="18"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -862,7 +862,7 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="9"/>
@@ -873,7 +873,7 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A6" s="26"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -888,14 +888,14 @@
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="28" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
@@ -907,14 +907,14 @@
       <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14">
         <v>45</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="7">
         <v>135</v>
       </c>
@@ -926,14 +926,14 @@
       <c r="B9" s="4">
         <v>23</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22">
+      <c r="D9" s="13"/>
+      <c r="E9" s="14">
         <v>4</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="7">
         <v>92</v>
       </c>
@@ -941,50 +941,50 @@
     <row r="10" spans="1:7" ht="11.25" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="11.25" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="11.25" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="11.25" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="11.25" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="11.25" customHeight="1">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="9"/>
@@ -998,7 +998,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="11.25" customHeight="1">
-      <c r="A16" s="33"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1007,7 +1007,7 @@
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="9"/>
@@ -1021,7 +1021,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="9"/>
@@ -1032,27 +1032,27 @@
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="11.25" customHeight="1">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" ht="11.25" customHeight="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" ht="10.5" customHeight="1">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="9"/>
@@ -1063,7 +1063,7 @@
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="24" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="9"/>
@@ -1076,7 +1076,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="9"/>
@@ -2044,24 +2044,11 @@
     <row r="976" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A19:G20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:G3"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
@@ -2071,11 +2058,24 @@
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A15:F15"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>